<commit_message>
feat: introducing scripts for 3 pages
</commit_message>
<xml_diff>
--- a/extract_list/outputs/amazonbr-suplementos.xlsx
+++ b/extract_list/outputs/amazonbr-suplementos.xlsx
@@ -952,7 +952,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6337"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>